<commit_message>
add en el objeto de product-url, product-img y add oncity en el scraping
</commit_message>
<xml_diff>
--- a/busqueda.xlsx
+++ b/busqueda.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\proyectos\test-playwright-js\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\proyectos\api-scraping-ymk\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>l32s5400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Smart tv android tcl 32 fhdsmart tv-rv l32s5400-f </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID_FRABRICANTE</t>
   </si>
@@ -38,67 +32,19 @@
     <t>NOMBRES_DEL_ARTICULO</t>
   </si>
   <si>
-    <t>DAID550K</t>
-  </si>
-  <si>
-    <t>KIT TALADRO DAEWOO - 550W - PERCUTOR, -INCLUYE ACCESORIOS- NARANJA - DAID550K</t>
-  </si>
-  <si>
-    <t>8637F</t>
-  </si>
-  <si>
-    <t>COCINA ELECTRICA FLORENCIA - 56CM VITROCERAMICO H/CONVECTOR - NEGRA - FLOR 8637F</t>
-  </si>
-  <si>
     <t>PVP</t>
   </si>
   <si>
-    <t>$ 368.990</t>
-  </si>
-  <si>
-    <t>$ 101.390</t>
-  </si>
-  <si>
-    <t>$ 1.073.290</t>
-  </si>
-  <si>
-    <t>Af2090</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freidora Smart Tek Digital 9 Lts 2400W Af2090 </t>
-  </si>
-  <si>
-    <t>$ 237.890</t>
-  </si>
-  <si>
     <t>COSTO_ACTUAL</t>
   </si>
   <si>
     <t>UTILIDAD</t>
   </si>
   <si>
-    <t>mf200d80wb/t-a1</t>
-  </si>
-  <si>
-    <t>rt29k577js8</t>
-  </si>
-  <si>
-    <t>kjhaf1001</t>
-  </si>
-  <si>
-    <t>em6603ss</t>
-  </si>
-  <si>
     <t>Hp8321</t>
   </si>
   <si>
     <t>Planchita Philips Hp8321/00 Negra</t>
-  </si>
-  <si>
-    <t>hd9368</t>
-  </si>
-  <si>
-    <t>Pava electrica Philips 1.7L control de temperatura blanca - hd9368/00</t>
   </si>
 </sst>
 </file>
@@ -432,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,146 +394,31 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>